<commit_message>
Update the slider tooltip to enable the arrow to control the slider values
</commit_message>
<xml_diff>
--- a/data/story.xlsx
+++ b/data/story.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI AI intake 44\13- Visualization\Dashboard Project\Space-App-master\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\ITI\Data Visualization\project\Story-of-Palestine-Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E5CD92-5B32-44B5-AB02-DF6A94A0E2A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39432B8-DC9F-4FB2-AF8C-E945E23AC337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="20250" windowHeight="10920" xr2:uid="{EE290E89-57FC-4282-8650-4D083D184ED8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EE290E89-57FC-4282-8650-4D083D184ED8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
   <si>
     <t>year</t>
   </si>
@@ -940,6 +940,9 @@
   <si>
     <t>Israel announced the legendary right of return that any Jew has the right to return to 
 Israel. Israel that represents the extension of the Jewish state after the roman invasion in 70 B.C., 2000 years ago! It's actually ironic: Why would someone who never lived on this land has the right to return to it? while someone who actually lived on the land doesn't have the right to return? The only condition for Israel's return law is to have a Jewish mother.</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -1148,9 +1151,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1188,7 +1191,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1294,7 +1297,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1436,7 +1439,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1444,805 +1447,910 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A4C8C9-298F-45C5-A7B2-E7118898EDAA}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="32" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="32" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="H1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="114" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+    <row r="2" spans="1:11" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15">
         <v>1897</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="C2" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="D2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="15"/>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
-    </row>
-    <row r="3" spans="1:10" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="K2" s="15"/>
+    </row>
+    <row r="3" spans="1:11" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15">
         <v>1907</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="15"/>
+      <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="I3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="15"/>
       <c r="J3" s="15"/>
-    </row>
-    <row r="4" spans="1:10" ht="146.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+      <c r="K3" s="15"/>
+    </row>
+    <row r="4" spans="1:11" ht="146.25" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="15">
         <v>1910</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="15"/>
+      <c r="D4" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="15"/>
       <c r="G4" s="15"/>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="15"/>
+      <c r="I4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="15"/>
       <c r="J4" s="15"/>
-    </row>
-    <row r="5" spans="1:10" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
+      <c r="K4" s="15"/>
+    </row>
+    <row r="5" spans="1:11" ht="101.25" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="15">
         <v>1915</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="C5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="F5" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
-    </row>
-    <row r="6" spans="1:10" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="15">
         <v>1917</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="D6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="F6" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
-    </row>
-    <row r="7" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15">
         <v>1920</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="15"/>
+      <c r="D7" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="F7" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="4" t="s">
+      <c r="G7" s="1"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="J7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="15"/>
-    </row>
-    <row r="8" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="K7" s="15"/>
+    </row>
+    <row r="8" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="15">
         <v>1921</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="15"/>
+      <c r="D8" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="F8" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
-    </row>
-    <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="K8" s="15"/>
+    </row>
+    <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="15">
         <v>1922</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="15"/>
+      <c r="D9" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="F9" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="F9" s="13"/>
       <c r="G9" s="13"/>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="13"/>
+      <c r="I9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I9" s="15"/>
       <c r="J9" s="15"/>
-    </row>
-    <row r="10" spans="1:10" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+      <c r="K9" s="15"/>
+    </row>
+    <row r="10" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="15">
         <v>1929</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="F10" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="G10" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="15"/>
+      <c r="I10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="J10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J10" s="15"/>
-    </row>
-    <row r="11" spans="1:10" ht="187.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" spans="1:11" ht="187.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="15">
         <v>1935</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="F11" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4" t="s">
+      <c r="G11" s="15"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="15"/>
       <c r="J11" s="15"/>
-    </row>
-    <row r="12" spans="1:10" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="1:11" ht="168.75" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="15">
         <v>1936</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="15"/>
+      <c r="D12" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="E12" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="F12" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="F12" s="15"/>
       <c r="G12" s="15"/>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="15"/>
+      <c r="I12" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="15"/>
       <c r="J12" s="15"/>
-    </row>
-    <row r="13" spans="1:10" ht="135" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
+      <c r="K12" s="15"/>
+    </row>
+    <row r="13" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="15">
         <v>1937</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="15"/>
+      <c r="D13" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="F13" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="F13" s="15"/>
       <c r="G13" s="15"/>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="15"/>
+      <c r="I13" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="I13" s="15"/>
       <c r="J13" s="15"/>
-    </row>
-    <row r="14" spans="1:10" ht="126" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
+      <c r="K13" s="15"/>
+    </row>
+    <row r="14" spans="1:11" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="15">
         <v>1938</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="15"/>
+      <c r="D14" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="F14" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="F14" s="15"/>
       <c r="G14" s="15"/>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="15"/>
+      <c r="I14" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="I14" s="15"/>
       <c r="J14" s="15"/>
-    </row>
-    <row r="15" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="15">
+      <c r="K14" s="15"/>
+    </row>
+    <row r="15" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="15">
         <v>1939</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="15"/>
+      <c r="D15" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="F15" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="F15" s="15"/>
       <c r="G15" s="15"/>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="15"/>
+      <c r="I15" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="I15" s="15"/>
       <c r="J15" s="15"/>
-    </row>
-    <row r="16" spans="1:10" ht="144" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15">
+      <c r="K15" s="15"/>
+    </row>
+    <row r="16" spans="1:11" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="15">
         <v>1942</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="15"/>
+      <c r="D16" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="F16" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="F16" s="15"/>
       <c r="G16" s="15"/>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="15"/>
+      <c r="I16" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I16" s="15"/>
       <c r="J16" s="15"/>
-    </row>
-    <row r="17" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
+      <c r="K16" s="15"/>
+    </row>
+    <row r="17" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="15">
         <v>1946</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="15"/>
+      <c r="D17" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="F17" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="F17" s="15"/>
       <c r="G17" s="15"/>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="15"/>
+      <c r="I17" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I17" s="15"/>
       <c r="J17" s="15"/>
-    </row>
-    <row r="18" spans="1:10" ht="196.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15">
+      <c r="K17" s="15"/>
+    </row>
+    <row r="18" spans="1:11" ht="196.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="15">
         <v>1947</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="C18" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="D18" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="F18" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="F18" s="15"/>
       <c r="G18" s="15"/>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="15"/>
+      <c r="I18" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I18" s="15"/>
       <c r="J18" s="15"/>
-    </row>
-    <row r="19" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" s="15">
+      <c r="K18" s="15"/>
+    </row>
+    <row r="19" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="15">
         <v>1947</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="C19" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="D19" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="F19" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="F19" s="15"/>
       <c r="G19" s="15"/>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="15"/>
+      <c r="I19" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="I19" s="15"/>
       <c r="J19" s="15"/>
-    </row>
-    <row r="20" spans="1:10" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="15">
+      <c r="K19" s="15"/>
+    </row>
+    <row r="20" spans="1:11" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="15">
         <v>1948</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="C20" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="D20" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="F20" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="F20" s="15"/>
       <c r="G20" s="15"/>
-      <c r="H20" s="15" t="s">
+      <c r="H20" s="15"/>
+      <c r="I20" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="I20" s="15"/>
       <c r="J20" s="15"/>
-    </row>
-    <row r="21" spans="1:10" ht="168.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="15">
+      <c r="K20" s="15"/>
+    </row>
+    <row r="21" spans="1:11" ht="168.75" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="15">
         <v>1948</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="15"/>
+      <c r="D21" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="E21" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="F21" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="F21" s="15"/>
       <c r="G21" s="15"/>
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="15"/>
+      <c r="I21" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I21" s="15"/>
       <c r="J21" s="15"/>
-    </row>
-    <row r="22" spans="1:10" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="15">
+      <c r="K21" s="15"/>
+    </row>
+    <row r="22" spans="1:11" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="15">
         <v>1949</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="15"/>
+      <c r="D22" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="F22" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F22" s="15"/>
       <c r="G22" s="15"/>
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="15"/>
+      <c r="I22" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="I22" s="15"/>
       <c r="J22" s="15"/>
-    </row>
-    <row r="23" spans="1:10" ht="123.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="15">
+      <c r="K22" s="15"/>
+    </row>
+    <row r="23" spans="1:11" ht="123.75" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="15">
         <v>1950</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="15"/>
+      <c r="D23" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="E23" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="F23" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
-    </row>
-    <row r="24" spans="1:10" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="15">
+      <c r="K23" s="15"/>
+    </row>
+    <row r="24" spans="1:11" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="15">
         <v>1967</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="15"/>
+      <c r="D24" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="E24" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="F24" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="11" t="s">
+      <c r="H24" s="15"/>
+      <c r="I24" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="I24" s="15"/>
       <c r="J24" s="15"/>
-    </row>
-    <row r="25" spans="1:10" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="15">
+      <c r="K24" s="15"/>
+    </row>
+    <row r="25" spans="1:11" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="15">
         <v>1973</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="15"/>
+      <c r="D25" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="E25" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="F25" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="F25" s="15"/>
       <c r="G25" s="15"/>
-      <c r="H25" s="4" t="s">
+      <c r="H25" s="15"/>
+      <c r="I25" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I25" s="15"/>
       <c r="J25" s="15"/>
-    </row>
-    <row r="26" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="15">
+      <c r="K25" s="15"/>
+    </row>
+    <row r="26" spans="1:11" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="15">
         <v>1974</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="15"/>
+      <c r="D26" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="E26" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="F26" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="F26" s="15"/>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
-    </row>
-    <row r="27" spans="1:10" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="15">
+      <c r="K26" s="15"/>
+    </row>
+    <row r="27" spans="1:11" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="15">
         <v>1987</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="15"/>
+      <c r="D27" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="F27" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="F27" s="15"/>
       <c r="G27" s="15"/>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="15"/>
+      <c r="I27" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="I27" s="15"/>
       <c r="J27" s="15"/>
-    </row>
-    <row r="28" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
+      <c r="K27" s="15"/>
+    </row>
+    <row r="28" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="15">
         <v>1993</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="15"/>
+      <c r="D28" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="E28" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="F28" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="F28" s="15"/>
       <c r="G28" s="15"/>
-      <c r="H28" s="19" t="s">
+      <c r="H28" s="15"/>
+      <c r="I28" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="I28" s="15"/>
       <c r="J28" s="15"/>
-    </row>
-    <row r="29" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="15">
+      <c r="K28" s="15"/>
+    </row>
+    <row r="29" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="15">
         <v>2000</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="15"/>
+      <c r="D29" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="F29" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
-    </row>
-    <row r="30" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="15">
+      <c r="K29" s="15"/>
+    </row>
+    <row r="30" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="15">
         <v>2005</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="15"/>
+      <c r="D30" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="E30" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E30" s="13" t="s">
+      <c r="F30" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F30" s="15"/>
       <c r="G30" s="15"/>
-      <c r="H30" s="20" t="s">
+      <c r="H30" s="15"/>
+      <c r="I30" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="I30" s="15"/>
       <c r="J30" s="15"/>
-    </row>
-    <row r="31" spans="1:10" ht="57" x14ac:dyDescent="0.25">
-      <c r="A31" s="15">
+      <c r="K30" s="15"/>
+    </row>
+    <row r="31" spans="1:11" ht="57" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="15">
         <v>2006</v>
       </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="15"/>
+      <c r="D31" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="F31" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F31" s="15"/>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
-    </row>
-    <row r="32" spans="1:10" ht="135" x14ac:dyDescent="0.25">
-      <c r="A32" s="15">
+      <c r="K31" s="15"/>
+    </row>
+    <row r="32" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="15">
         <v>2008</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="15"/>
+      <c r="D32" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="E32" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="E32" s="13" t="s">
+      <c r="F32" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="F32" s="15"/>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
-    </row>
-    <row r="33" spans="1:10" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="15">
+      <c r="K32" s="15"/>
+    </row>
+    <row r="33" spans="1:11" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="15">
         <v>2014</v>
       </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="15"/>
+      <c r="D33" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="E33" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E33" s="13" t="s">
+      <c r="F33" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="F33" s="15"/>
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
       <c r="J33" s="15"/>
-    </row>
-    <row r="34" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="15">
+      <c r="K33" s="15"/>
+    </row>
+    <row r="34" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="15">
         <v>2021</v>
       </c>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="15"/>
+      <c r="D34" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="E34" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="E34" s="13" t="s">
+      <c r="F34" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="F34" s="15"/>
       <c r="G34" s="15"/>
-      <c r="H34" s="13" t="s">
+      <c r="H34" s="15"/>
+      <c r="I34" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="I34" s="15"/>
       <c r="J34" s="15"/>
-    </row>
-    <row r="35" spans="1:10" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="15">
+      <c r="K34" s="15"/>
+    </row>
+    <row r="35" spans="1:11" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="15">
         <v>2023</v>
       </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="15"/>
+      <c r="D35" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="E35" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E35" s="13" t="s">
+      <c r="F35" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="F35" s="15"/>
       <c r="G35" s="15"/>
-      <c r="H35" s="4" t="s">
+      <c r="H35" s="15"/>
+      <c r="I35" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="I35" s="15"/>
       <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Hover text on image functionality added
</commit_message>
<xml_diff>
--- a/data/story.xlsx
+++ b/data/story.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\ITI\Data Visualization\project\Story-of-Palestine-Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39432B8-DC9F-4FB2-AF8C-E945E23AC337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826542D0-5066-4425-A060-877F93B19B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EE290E89-57FC-4282-8650-4D083D184ED8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="151">
   <si>
     <t>year</t>
   </si>
@@ -943,6 +943,9 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
@@ -1449,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A4C8C9-298F-45C5-A7B2-E7118898EDAA}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32:I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1521,7 +1524,9 @@
       <c r="H2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="15"/>
+      <c r="I2" s="15" t="s">
+        <v>150</v>
+      </c>
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
     </row>
@@ -1600,7 +1605,9 @@
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
+      <c r="I5" s="15" t="s">
+        <v>150</v>
+      </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
     </row>
@@ -1625,7 +1632,9 @@
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
+      <c r="I6" s="15" t="s">
+        <v>150</v>
+      </c>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
     </row>
@@ -1675,7 +1684,9 @@
       </c>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
+      <c r="I8" s="15" t="s">
+        <v>150</v>
+      </c>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
     </row>
@@ -2058,7 +2069,9 @@
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
+      <c r="I23" s="15" t="s">
+        <v>150</v>
+      </c>
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
     </row>
@@ -2204,7 +2217,9 @@
       </c>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
+      <c r="I29" s="15" t="s">
+        <v>150</v>
+      </c>
       <c r="J29" s="15"/>
       <c r="K29" s="15"/>
     </row>
@@ -2252,7 +2267,9 @@
       </c>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
+      <c r="I31" s="15" t="s">
+        <v>150</v>
+      </c>
       <c r="J31" s="15"/>
       <c r="K31" s="15"/>
     </row>
@@ -2275,7 +2292,9 @@
       </c>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
+      <c r="I32" s="15" t="s">
+        <v>150</v>
+      </c>
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
     </row>
@@ -2298,7 +2317,9 @@
       </c>
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
+      <c r="I33" s="15" t="s">
+        <v>150</v>
+      </c>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
     </row>

</xml_diff>

<commit_message>
Update story - adding some pictuers
</commit_message>
<xml_diff>
--- a/data/story.xlsx
+++ b/data/story.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\ITI\Data Visualization\project\Story-of-Palestine-Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826542D0-5066-4425-A060-877F93B19B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B170162-4639-4059-8FF2-822F0ACE85B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EE290E89-57FC-4282-8650-4D083D184ED8}"/>
+    <workbookView xWindow="-28920" yWindow="-6720" windowWidth="29040" windowHeight="15840" xr2:uid="{EE290E89-57FC-4282-8650-4D083D184ED8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
   <si>
     <t>year</t>
   </si>
@@ -235,9 +235,84 @@
     <t>Nakba</t>
   </si>
   <si>
-    <r>
-      <t>The </t>
-    </r>
+    <t>Plan Dalet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A complete ethnic cleansing plan on paper is ready to go. However, it needs a real trial, a rehearsal. The rehearsal took place on February 15th, 1948. When the Palmach leader Yitzhak Rabin, who was awarded a Nobel prize for peace by the way, led an attack on the village of Caesarea in Haifa district expelling 1500 of its inhabitants. The Zionists attacked 5 villages to ensure the efficiency of their fighters. And to make sure that the remaining British soldiers who haven't left yet won't intervene. The gangs start an organized attack on the villages surrounding Jerusalem. </t>
+  </si>
+  <si>
+    <t>Right Of Return</t>
+  </si>
+  <si>
+    <t>The UN issued Resolution 194 guaranteeing the right of return for every refugee who was expelled. refugees' number went up to 5 million refugees. The Argentinian researcher Pedro Brieger, during his visit to refugee camps decades after the Nakba, found that all children introduce themselves with names of the villages that their ancestors were expelled from. He still has the key of his grandparents' house that they were kicked from. Generations would still pass on these keys, one to another. The right of return that the UN  granted the Palestinians in 1949 as you know, was never implemented.</t>
+  </si>
+  <si>
+    <t>Right Of Return1.jpg</t>
+  </si>
+  <si>
+    <t>A Palestinian refugee, Saleh Saleh Abu Rass, holds up a key from his original home in Be’er Sheva, located in southern Israel, during a rally, in Rafah refugee camp, southern Gaza Strip, May 12, 2013. (Abed Rahim Khatib/Flash 90)</t>
+  </si>
+  <si>
+    <t>legendary Right Of Return</t>
+  </si>
+  <si>
+    <t>Six-Day War</t>
+  </si>
+  <si>
+    <t>Israel gains control of the West Bank, Gaza Strip, Sinai Peninsula, and Golan Heights following a preemptive strike against Egypt, Jordan, and Syria.</t>
+  </si>
+  <si>
+    <t>October War</t>
+  </si>
+  <si>
+    <t>Israel and Egypt sign peace treaty, Israel withdraws from Sinai.</t>
+  </si>
+  <si>
+    <t>Camp David</t>
+  </si>
+  <si>
+    <t>legendary Right Of Return1.jpg</t>
+  </si>
+  <si>
+    <t>Zionist prisoners wearing Egyptian Castor pajamas after their release and arrival at a hospital in Tel Aviv after the end of the October 1973 war.</t>
+  </si>
+  <si>
+    <t>Oslo Accords</t>
+  </si>
+  <si>
+    <t>Oslo Accords1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Israel and PLO sign agreements aimed at achieving peace and Palestinian self-governance</t>
+  </si>
+  <si>
+    <t>Second Intifada</t>
+  </si>
+  <si>
+    <t>The Second Intifada started on 28 September 2000, after Ariel Sharon, a Likud party candidate for Israeli Prime Minister, made a visit to the Temple Mount, also known as Al-Haram Al-Sharif, an area sacred to both Jews and Muslims, accompanied by over 1,000 security guards.</t>
+  </si>
+  <si>
+    <t>Second Intifada1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaza Disengagement	</t>
+  </si>
+  <si>
+    <t>Gaza Disengagement1.jpg</t>
+  </si>
+  <si>
+    <t>Map of the Gaza Strip in May 2005, a few months prior to the Israeli withdrawal. The major settlement blocs were the blue-shaded regions of this map.</t>
+  </si>
+  <si>
+    <t>Hamas Victory in Palestinian Elections</t>
+  </si>
+  <si>
+    <t>Hamas Victory in Palestinian Elections1.jpg</t>
+  </si>
+  <si>
+    <t>Operation Cast Lead</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -246,7 +321,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Nakba</t>
+      <t xml:space="preserve">Operation Cast Lead </t>
     </r>
     <r>
       <rPr>
@@ -255,7 +330,26 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> was the </t>
+      <t>also known as the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Gaza Massacre</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> It was a three-week armed conflict between </t>
     </r>
     <r>
       <rPr>
@@ -264,7 +358,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>ethnic cleansing</t>
+      <t>Gaza Strip</t>
     </r>
     <r>
       <rPr>
@@ -273,7 +367,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t> of </t>
+      <t> Palestinian paramilitary groups and the </t>
     </r>
     <r>
       <rPr>
@@ -282,7 +376,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Palestinians</t>
+      <t>Israel Defense Forces</t>
     </r>
     <r>
       <rPr>
@@ -291,7 +385,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t> in </t>
+      <t> (IDF) that </t>
     </r>
     <r>
       <rPr>
@@ -300,7 +394,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Mandatory Palestine</t>
+      <t>began</t>
     </r>
     <r>
       <rPr>
@@ -309,359 +403,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t> during the </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF3366CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>1948 Palestine War</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> through their </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF3366CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>violent displacement</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> and dispossession of land, property, and belongings, along with the destruction of their society, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF3366CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>culture</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF3366CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>identity</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, political rights, and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF3366CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>national aspirations</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF3366CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[2]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> The term is also used to describe the </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF3366CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ongoing persecution and displacement</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> of Palestinians by </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF3366CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Israel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>. As a whole, it covers the shattering of Palestinian society and the long-running rejection of the </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF3366CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>right of return</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> for </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF3366CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Palestinian refugees and their descendants.</t>
-    </r>
-  </si>
-  <si>
-    <t>Plan Dalet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A complete ethnic cleansing plan on paper is ready to go. However, it needs a real trial, a rehearsal. The rehearsal took place on February 15th, 1948. When the Palmach leader Yitzhak Rabin, who was awarded a Nobel prize for peace by the way, led an attack on the village of Caesarea in Haifa district expelling 1500 of its inhabitants. The Zionists attacked 5 villages to ensure the efficiency of their fighters. And to make sure that the remaining British soldiers who haven't left yet won't intervene. The gangs start an organized attack on the villages surrounding Jerusalem. </t>
-  </si>
-  <si>
-    <t>Right Of Return</t>
-  </si>
-  <si>
-    <t>The UN issued Resolution 194 guaranteeing the right of return for every refugee who was expelled. refugees' number went up to 5 million refugees. The Argentinian researcher Pedro Brieger, during his visit to refugee camps decades after the Nakba, found that all children introduce themselves with names of the villages that their ancestors were expelled from. He still has the key of his grandparents' house that they were kicked from. Generations would still pass on these keys, one to another. The right of return that the UN  granted the Palestinians in 1949 as you know, was never implemented.</t>
-  </si>
-  <si>
-    <t>Right Of Return1.jpg</t>
-  </si>
-  <si>
-    <t>A Palestinian refugee, Saleh Saleh Abu Rass, holds up a key from his original home in Be’er Sheva, located in southern Israel, during a rally, in Rafah refugee camp, southern Gaza Strip, May 12, 2013. (Abed Rahim Khatib/Flash 90)</t>
-  </si>
-  <si>
-    <t>legendary Right Of Return</t>
-  </si>
-  <si>
-    <t>Six-Day War</t>
-  </si>
-  <si>
-    <t>Israel gains control of the West Bank, Gaza Strip, Sinai Peninsula, and Golan Heights following a preemptive strike against Egypt, Jordan, and Syria.</t>
-  </si>
-  <si>
-    <t>October War</t>
-  </si>
-  <si>
-    <t>Israel and Egypt sign peace treaty, Israel withdraws from Sinai.</t>
-  </si>
-  <si>
-    <t>Camp David</t>
-  </si>
-  <si>
-    <t>legendary Right Of Return1.jpg</t>
-  </si>
-  <si>
-    <t>Zionist prisoners wearing Egyptian Castor pajamas after their release and arrival at a hospital in Tel Aviv after the end of the October 1973 war.</t>
-  </si>
-  <si>
-    <t>Oslo Accords</t>
-  </si>
-  <si>
-    <t>Oslo Accords1.jpg</t>
-  </si>
-  <si>
-    <t>Widespread protests and resistance against Israeli occupation erupt in the occupied territories.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Israel and PLO sign agreements aimed at achieving peace and Palestinian self-governance</t>
-  </si>
-  <si>
-    <t>Second Intifada</t>
-  </si>
-  <si>
-    <t>The Second Intifada started on 28 September 2000, after Ariel Sharon, a Likud party candidate for Israeli Prime Minister, made a visit to the Temple Mount, also known as Al-Haram Al-Sharif, an area sacred to both Jews and Muslims, accompanied by over 1,000 security guards.</t>
-  </si>
-  <si>
-    <t>Second Intifada1.jpg</t>
-  </si>
-  <si>
-    <t>The disengagement was proposed in 2003 by Prime Minister Ariel Sharon, adopted by the government in June 2004, and approved by the Knesset in February 2005 as the Disengagement Plan Implementation Law.[2] It was implemented in August 2005 and completed in September 2005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gaza Disengagement	</t>
-  </si>
-  <si>
-    <t>Gaza Disengagement1.jpg</t>
-  </si>
-  <si>
-    <t>Map of the Gaza Strip in May 2005, a few months prior to the Israeli withdrawal. The major settlement blocs were the blue-shaded regions of this map.</t>
-  </si>
-  <si>
-    <t>Hamas Victory in Palestinian Elections</t>
-  </si>
-  <si>
-    <t>Hamas wins Palestinian legislative elections.</t>
-  </si>
-  <si>
-    <t>Hamas Victory in Palestinian Elections1.jpg</t>
-  </si>
-  <si>
-    <t>Operation Cast Lead</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Operation Cast Lead </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>also known as the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Gaza Massacre</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> It was a three-week armed conflict between </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF3366CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Gaza Strip</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> Palestinian paramilitary groups and the </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF3366CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Israel Defense Forces</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> (IDF) that </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF3366CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>began</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t> on 27 December 2008 and ended on 18 January 2009 with a unilateral ceasefire. The conflict resulted in 1,166–1,417 Palestinian and 13 Israeli deaths. Over 46,000 homes were destroyed in Gaza, making more than 100,000 people homeless.</t>
     </r>
   </si>
@@ -754,9 +495,6 @@
   </si>
   <si>
     <t>British Officers' Club1.jpg</t>
-  </si>
-  <si>
-    <t>Partition Resolution 1811.webp</t>
   </si>
   <si>
     <t>Plan Dalet1.jpg</t>
@@ -858,83 +596,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Israeli prime minister </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF3366CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Yitzhak Rabin</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> (left), American president </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF3366CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Bill Clinton</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> (middle), and Palestinian political leader </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF3366CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Yasser Arafat</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> (right) at the </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF3366CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>White House</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> in 1993</t>
-    </r>
-  </si>
-  <si>
     <t> Palestinian protests began on 6 May in Sheikh Jarrah, but clashes soon spread to the al-Aqsa Mosque, Lod, other Arab localities in Israel, and the West Bank. Between 10 and 14 May Israeli security inflicted injuries on approximately 1,000 Palestinian protesters in East Jerusalem.</t>
   </si>
   <si>
@@ -945,7 +606,367 @@
     <t>id</t>
   </si>
   <si>
-    <t>NULL</t>
+    <t>First Zionist Congress with Theodor Herzl</t>
+  </si>
+  <si>
+    <t>From left, Lords Edmund Allenby, Arthur Balfour and Sir Herbert Samuel, at Hebrew University in 1925.</t>
+  </si>
+  <si>
+    <t>The original letter from Balfour to Rothschild; the declaration reads:
+His Majesty's Government view with favour the establishment in Palestine of a national home for the Jewish people, and will use their best endeavours to facilitate the achievement of this object, it being clearly understood that nothing shall be done which may prejudice the civil and religious rights of existing non-Jewish communities in Palestine, or the rights and political status enjoyed by Jews in any other country.</t>
+  </si>
+  <si>
+    <t>The arrival of the ship "Roslin" in the port of Jaffa on December 19, 1919, symbolized the beginning of the third wave of Jewish immigration to Palestine from Europe between 1919 and 1923 (from the end of World War I until the beginning of the economic crisis in the country).</t>
+  </si>
+  <si>
+    <t>Partition Resolution 1811.jpg</t>
+  </si>
+  <si>
+    <t>Jewish immigrants arriving in Israel under the Law of Return, 1954</t>
+  </si>
+  <si>
+    <t>U.S. Pres. Jimmy Carter (second from left), occupation Prime Minister Menachem Begin (left), and Egyptian Pres. Anwar Sadat clasping hands on the White House lawn after the signing of the peace treaty, March 26, 1979.</t>
+  </si>
+  <si>
+    <t>Widespread protests and resistance against occupation erupt in the occupied territories. The intifada began on December 9 1987, in the Jabalia refugee camp after an Israeli truck driver collided with a civilian car, killing four Palestinian workers, three of whom were from the Jabalia refugee camp. Palestinians charged that the collision was a deliberate response to the killing of an Israeli in Gaza days earlier.</t>
+  </si>
+  <si>
+    <r>
+      <t>occupation prime minister </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF3366CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Yitzhak Rabin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (left), American president </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF3366CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bill Clinton</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (middle), and Palestinian political leader </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF3366CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Yasser Arafat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (right) at the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF3366CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>White House</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> in 1993</t>
+    </r>
+  </si>
+  <si>
+    <t>Israeli troops run as clashes erupt outside the Al-Aqsa mosque compound in Jerusalem’s Old City 28 September 2000.</t>
+  </si>
+  <si>
+    <t>The disengagement was proposed in 2003 by Prime Minister Ariel Sharon, adopted by the government in June 2004, and approved by the Knesset in February 2005 as the Disengagement Plan Implementation Law. It was implemented in August 2005 and completed in September 2005</t>
+  </si>
+  <si>
+    <t>Legislative elections were held in the Palestinian territories on 25 January 2006 in order to elect the second Palestinian Legislative Council (PLC), the legislature of the Palestinian National Authority (PNA). The result was a victory for Hamas, contesting under the list name of Change and Reform, which received 44.45% of the vote and won 74 of the 132 seats, whilst the ruling Fatah received 41.43% of the vote and won 45 seats.</t>
+  </si>
+  <si>
+    <t>celebrations Hamas wins Palestinian legislative elections.</t>
+  </si>
+  <si>
+    <t>occupation using white phosphorus as a weapon of terror against innocent Palestinians in Gaza 2008.</t>
+  </si>
+  <si>
+    <t>The presence of Jews in the Jerusalem Day demonstrations in Berlin, Germany, in 2014. supporting Palestinians against zionist terrorism.</t>
+  </si>
+  <si>
+    <r>
+      <t>The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nakba</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> was the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF3366CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ethnic cleansing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF3366CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Palestinians</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF3366CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Mandatory Palestine</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> during the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF3366CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1948 Palestine War</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> through their </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF3366CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>violent displacement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> and dispossession of land, property, and belongings, along with the destruction of their society, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF3366CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>culture</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF3366CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>identity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, political rights, and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF3366CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>national aspirations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>. The term is also used to describe the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF3366CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ongoing persecution and displacement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> of Palestinians by </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF3366CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Israel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>. As a whole, it covers the shattering of Palestinian society and the long-running rejection of the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF3366CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>right of return</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF3366CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Palestinian refugees and their descendants.</t>
+    </r>
+  </si>
+  <si>
+    <t>Nearly 500 people have been killed in an Israeli air attack on the al-Ahli Arab Hospital in the besieged Gaza Strip. No doubt that the IDF is targeting civilians despite many pro-Israeli media claiming that the IDF is not responsible for targeting the hospital. many world leaders condemned this act of targeting civilians and hospitals including French President Emmanuel Macron, China’s foreign ministry, famous football player Mohamed Salah, and many more. Yet the Zionist terrorism is still active and targeting more civilians and kids until now……………</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bombing of Al-Mamadani Hospital </t>
+  </si>
+  <si>
+    <t>20240427_012432.jpg</t>
+  </si>
+  <si>
+    <t>Ziad Shehadah, a medical doctor, said, "What’s happened is terrible because those people, all of them, are civilians. They fled their homes and reached a place that they believed was safe — a hospital, which according to international law, is a safe place."</t>
   </si>
 </sst>
 </file>
@@ -1017,13 +1038,6 @@
       <family val="2"/>
     </font>
     <font>
-      <vertAlign val="superscript"/>
-      <sz val="8"/>
-      <color rgb="FF3366CC"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color rgb="FF202122"/>
       <name val="Arial"/>
@@ -1054,6 +1068,12 @@
       <name val="Georgia"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF595959"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1075,7 +1095,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1105,10 +1125,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1121,20 +1141,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1450,10 +1479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A4C8C9-298F-45C5-A7B2-E7118898EDAA}">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32:I33"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1466,7 +1495,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>0</v>
@@ -1507,7 +1536,7 @@
         <v>1897</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>4</v>
@@ -1516,7 +1545,7 @@
         <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>9</v>
@@ -1524,8 +1553,8 @@
       <c r="H2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="15" t="s">
-        <v>150</v>
+      <c r="I2" s="13" t="s">
+        <v>144</v>
       </c>
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
@@ -1545,10 +1574,10 @@
         <v>19</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>17</v>
@@ -1574,7 +1603,7 @@
         <v>20</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
@@ -1601,12 +1630,12 @@
         <v>21</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
-      <c r="I5" s="15" t="s">
-        <v>150</v>
+      <c r="I5" s="13" t="s">
+        <v>145</v>
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
@@ -1619,7 +1648,7 @@
         <v>1917</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>24</v>
@@ -1628,17 +1657,17 @@
         <v>25</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
-      <c r="I6" s="15" t="s">
-        <v>150</v>
+      <c r="I6" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
     </row>
-    <row r="7" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1653,7 +1682,7 @@
         <v>27</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="15"/>
@@ -1674,18 +1703,18 @@
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
-      <c r="I8" s="15" t="s">
-        <v>150</v>
+      <c r="I8" s="13" t="s">
+        <v>147</v>
       </c>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -1705,7 +1734,7 @@
         <v>32</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
@@ -1730,7 +1759,7 @@
         <v>36</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G10" s="13" t="s">
         <v>37</v>
@@ -1759,7 +1788,7 @@
         <v>39</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="4"/>
@@ -1769,7 +1798,7 @@
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
     </row>
-    <row r="12" spans="1:11" ht="168.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1784,7 +1813,7 @@
         <v>44</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
@@ -1809,12 +1838,12 @@
         <v>46</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
@@ -1834,12 +1863,12 @@
         <v>48</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
       <c r="I14" s="13" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
@@ -1859,12 +1888,12 @@
         <v>50</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
       <c r="I15" s="13" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
@@ -1884,7 +1913,7 @@
         <v>52</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
@@ -1909,7 +1938,7 @@
         <v>55</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
@@ -1927,7 +1956,7 @@
         <v>1947</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>57</v>
@@ -1936,7 +1965,7 @@
         <v>58</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
@@ -1954,7 +1983,7 @@
         <v>1947</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>60</v>
@@ -1963,7 +1992,7 @@
         <v>61</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
@@ -1981,21 +2010,21 @@
         <v>1948</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D20" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>66</v>
-      </c>
       <c r="F20" s="13" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
       <c r="I20" s="15" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
@@ -2012,15 +2041,15 @@
         <v>63</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
       <c r="I21" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
@@ -2034,18 +2063,18 @@
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="13" t="s">
         <v>68</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>69</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
       <c r="I22" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
@@ -2059,18 +2088,18 @@
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
-      <c r="I23" s="15" t="s">
-        <v>150</v>
+      <c r="I23" s="13" t="s">
+        <v>149</v>
       </c>
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
@@ -2084,18 +2113,18 @@
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="12" t="s">
-        <v>73</v>
-      </c>
       <c r="F24" s="13" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
       <c r="I24" s="11" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="J24" s="15"/>
       <c r="K24" s="15"/>
@@ -2109,23 +2138,23 @@
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
       <c r="I25" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J25" s="15"/>
       <c r="K25" s="15"/>
     </row>
-    <row r="26" spans="1:11" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="90.75" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2134,21 +2163,23 @@
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
+      <c r="I26" s="13" t="s">
+        <v>150</v>
+      </c>
       <c r="J26" s="15"/>
       <c r="K26" s="15"/>
     </row>
-    <row r="27" spans="1:11" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2157,18 +2188,18 @@
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="15" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>81</v>
+        <v>151</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
       <c r="I27" s="13" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="J27" s="15"/>
       <c r="K27" s="15"/>
@@ -2182,18 +2213,18 @@
       </c>
       <c r="C28" s="15"/>
       <c r="D28" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F28" s="13" t="s">
         <v>79</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="F28" s="13" t="s">
-        <v>80</v>
       </c>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
       <c r="I28" s="19" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="J28" s="15"/>
       <c r="K28" s="15"/>
@@ -2207,18 +2238,18 @@
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
-      <c r="I29" s="15" t="s">
-        <v>150</v>
+      <c r="I29" s="13" t="s">
+        <v>153</v>
       </c>
       <c r="J29" s="15"/>
       <c r="K29" s="15"/>
@@ -2232,23 +2263,23 @@
       </c>
       <c r="C30" s="15"/>
       <c r="D30" s="15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>86</v>
+        <v>154</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
       <c r="I30" s="20" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J30" s="15"/>
       <c r="K30" s="15"/>
     </row>
-    <row r="31" spans="1:11" ht="57" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="124.5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2257,18 +2288,18 @@
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>155</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
-      <c r="I31" s="15" t="s">
-        <v>150</v>
+      <c r="I31" s="22" t="s">
+        <v>156</v>
       </c>
       <c r="J31" s="15"/>
       <c r="K31" s="15"/>
@@ -2282,18 +2313,18 @@
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="15" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
-      <c r="I32" s="15" t="s">
-        <v>150</v>
+      <c r="I32" s="13" t="s">
+        <v>157</v>
       </c>
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
@@ -2307,18 +2338,18 @@
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
-      <c r="I33" s="15" t="s">
-        <v>150</v>
+      <c r="I33" s="13" t="s">
+        <v>158</v>
       </c>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
@@ -2332,18 +2363,18 @@
       </c>
       <c r="C34" s="15"/>
       <c r="D34" s="15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
       <c r="I34" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
@@ -2357,21 +2388,41 @@
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="13" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
       <c r="I35" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
+    </row>
+    <row r="36" spans="1:11" ht="146.25" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="15">
+        <v>2023</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="E36" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="I36" s="24" t="s">
+        <v>163</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Remove unnecessary columns from the story.xlsx
</commit_message>
<xml_diff>
--- a/data/story.xlsx
+++ b/data/story.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\ITI\Data Visualization\project\Story-of-Palestine-Dashboard\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI AI intake 44\13- Visualization\Dashboard Project\Space-App-master\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B170162-4639-4059-8FF2-822F0ACE85B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423FE488-2946-4375-8FE4-000AAC61CEFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-6720" windowWidth="29040" windowHeight="15840" xr2:uid="{EE290E89-57FC-4282-8650-4D083D184ED8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EE290E89-57FC-4282-8650-4D083D184ED8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
   <si>
     <t>year</t>
   </si>
@@ -44,9 +44,6 @@
     <t>event</t>
   </si>
   <si>
-    <t>month</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -59,39 +56,18 @@
     <t>picture1</t>
   </si>
   <si>
-    <t>picture2</t>
-  </si>
-  <si>
-    <t>picture3</t>
-  </si>
-  <si>
-    <t>First Zionist Congress2</t>
-  </si>
-  <si>
-    <t>First Zionist Congress3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chaim Weizmann company </t>
   </si>
   <si>
     <t>DIS1</t>
   </si>
   <si>
-    <t>DIS2</t>
-  </si>
-  <si>
-    <t>DIS3</t>
-  </si>
-  <si>
     <t>The inauguration of Chaim Weizmann AS Israel's First President</t>
   </si>
   <si>
     <t>Modern picture for Marj Ibn Amer</t>
   </si>
   <si>
-    <t>Chaim Weizmann company3</t>
-  </si>
-  <si>
     <t>Marj Ibn Amer</t>
   </si>
   <si>
@@ -107,9 +83,6 @@
     <t>Samuel secret document</t>
   </si>
   <si>
-    <t>Jan</t>
-  </si>
-  <si>
     <t>Balfour Declaration</t>
   </si>
   <si>
@@ -125,10 +98,6 @@
     <t>The front page of the Mandate for Palestine and Transjordan memorandum, presented to UK Parliament in December 1922, prior to it coming into force in 1923.</t>
   </si>
   <si>
-    <t>More details
-Herbert Samuel's proclamation in Salt on 21 August 1920 at the courtyard of the Assumption of Our Lady Catholic Church. Samuel was admonished a few days later by Curzon, who said: "There must be no question of setting up any British administration in that area".</t>
-  </si>
-  <si>
     <t>the Jewish migrations greatly increase. where 185,000 Jewish immigrants arrived, while the Jewish National Fund bought 240.000 acres from Jezreel Valley Northern of Palestine. With the idea of settlement turning into a full-scale European project, Violent demonstrations spread across Palestine starting from Jaffa, where 95 Jewish and 64 Arabs died.</t>
   </si>
   <si>
@@ -148,12 +117,6 @@
   </si>
   <si>
     <t>A Jewish prayer was organized in Jerusalem calling for the revival of the temple, and claims their historical right in the "Wailing Wall", which is called 'Buraq Wall' by Muslims. And the Jewish day of mourning the Temples destruction coincided with the Muslim Mawlid, so Palestinians got angry. That's the revolution we know as Buraq Uprising. When Palestinians were dismayed by the violent oppression led by the British. They didn't only arrest hundreds of rebels, they executed the uprising leaders.</t>
-  </si>
-  <si>
-    <t>Buraq Uprising2</t>
-  </si>
-  <si>
-    <t>The three Palestinians executed at Akka prison – Fouad Hijazi, Atta al-Zeer and Mohammed Khalil Jamjoum</t>
   </si>
   <si>
     <t>the Jewish immigrations continue. Until they reach 27% of the population in 1935. From 3% to 27%! And revolutions against them never stopped, revolutions against the unfair British colonization. And one of the major revolutionists was a Syrian guy from Al-Azhar University who turned from a preacher at the Istiqlal Mosque in Haifa to a leader of an armed movement against the British. His name is Izz al-Din al-Qassam. He was joined by thousands of volunteers who gave him ammunition and weapons. But, the occupation succeeded in Killing Izz al-Din al-Qassam in an unfair battle. Al-Qassam's funeral will turn into the heart of the people’s movement in Palestine. This movement turned later into a complete revolt from April to October of 1936.</t>
@@ -437,9 +400,6 @@
     <t>Chaim Weizmann company2.jpeg</t>
   </si>
   <si>
-    <t>Chaim Weizmann company1.jpg</t>
-  </si>
-  <si>
     <t>Marj Ibn Amer1.jpg</t>
   </si>
   <si>
@@ -538,21 +498,6 @@
   </si>
   <si>
     <t>People standing on a rooftop watch as a ball of fire and smoke rises above a building in Gaza City during an Israeli air strike that hit the Palestine Tower building</t>
-  </si>
-  <si>
-    <t>Aug</t>
-  </si>
-  <si>
-    <t>Nov</t>
-  </si>
-  <si>
-    <t>July</t>
-  </si>
-  <si>
-    <t>Feb</t>
-  </si>
-  <si>
-    <t>Sep</t>
   </si>
   <si>
     <r>
@@ -973,7 +918,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1016,13 +961,6 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="8"/>
-      <color rgb="FF444444"/>
-      <name val="Verdana"/>
       <family val="2"/>
     </font>
     <font>
@@ -1095,7 +1033,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1125,10 +1063,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1141,16 +1076,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1162,7 +1097,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1183,9 +1118,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1223,7 +1158,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1329,7 +1264,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1471,7 +1406,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1479,949 +1414,737 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A4C8C9-298F-45C5-A7B2-E7118898EDAA}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="32" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B1" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="15" t="s">
+      <c r="E1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="14">
         <v>1897</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="D2" s="15" t="s">
+      <c r="C2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-    </row>
-    <row r="3" spans="1:11" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="14">
         <v>1907</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-    </row>
-    <row r="4" spans="1:11" ht="146.25" x14ac:dyDescent="0.25">
+      <c r="E3" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="14">
         <v>1910</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-    </row>
-    <row r="5" spans="1:11" ht="101.25" x14ac:dyDescent="0.25">
+      <c r="C4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="101.25" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <v>1915</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-    </row>
-    <row r="6" spans="1:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>1917</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-    </row>
-    <row r="7" spans="1:11" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>1920</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" s="15"/>
-    </row>
-    <row r="8" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>1921</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-    </row>
-    <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="C8" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>1922</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-    </row>
-    <row r="10" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="C9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="14">
         <v>1929</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="K10" s="15"/>
-    </row>
-    <row r="11" spans="1:11" ht="187.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="187.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="14">
         <v>1935</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-    </row>
-    <row r="12" spans="1:11" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="C11" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="14">
         <v>1936</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-    </row>
-    <row r="13" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="C12" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="14">
         <v>1937</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-    </row>
-    <row r="14" spans="1:11" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="14">
         <v>1938</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-    </row>
-    <row r="15" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="C14" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="14">
         <v>1939</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-    </row>
-    <row r="16" spans="1:11" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="144" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="14">
         <v>1942</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-    </row>
-    <row r="17" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="C16" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="14">
         <v>1946</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-    </row>
-    <row r="18" spans="1:11" ht="196.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="196.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="14">
         <v>1947</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-    </row>
-    <row r="19" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="C18" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="14">
         <v>1947</v>
       </c>
-      <c r="C19" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-    </row>
-    <row r="20" spans="1:11" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="C19" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="14">
         <v>1948</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-    </row>
-    <row r="21" spans="1:11" ht="168.75" x14ac:dyDescent="0.25">
+      <c r="C20" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="168.75" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="14">
         <v>1948</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-    </row>
-    <row r="22" spans="1:11" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="C21" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="14">
         <v>1949</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-    </row>
-    <row r="23" spans="1:11" ht="123.75" x14ac:dyDescent="0.25">
+      <c r="C22" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="123.75" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="14">
         <v>1950</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-    </row>
-    <row r="24" spans="1:11" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="C23" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B24" s="14">
         <v>1967</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15" t="s">
-        <v>71</v>
+      <c r="C24" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-    </row>
-    <row r="25" spans="1:11" ht="157.5" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="14">
         <v>1973</v>
       </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="5" t="s">
-        <v>73</v>
+      <c r="C25" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-    </row>
-    <row r="26" spans="1:11" ht="90.75" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="90.75" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="14">
         <v>1974</v>
       </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="F26" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-    </row>
-    <row r="27" spans="1:11" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="C26" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="14">
         <v>1987</v>
       </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-    </row>
-    <row r="28" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="14">
         <v>1993</v>
       </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-    </row>
-    <row r="29" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="C28" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29" s="14">
         <v>2000</v>
       </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-    </row>
-    <row r="30" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="C29" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B30" s="14">
         <v>2005</v>
       </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-    </row>
-    <row r="31" spans="1:11" ht="124.5" x14ac:dyDescent="0.25">
+      <c r="C30" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="124.5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31" s="14">
         <v>2006</v>
       </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-    </row>
-    <row r="32" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="C31" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="15">
+      <c r="B32" s="14">
         <v>2008</v>
       </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F32" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-    </row>
-    <row r="33" spans="1:11" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="C32" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="15">
+      <c r="B33" s="14">
         <v>2014</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F33" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-    </row>
-    <row r="34" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="C33" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="15">
+      <c r="B34" s="14">
         <v>2021</v>
       </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F34" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-    </row>
-    <row r="35" spans="1:11" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="C34" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="15">
+      <c r="B35" s="14">
         <v>2023</v>
       </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F35" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-    </row>
-    <row r="36" spans="1:11" ht="146.25" x14ac:dyDescent="0.25">
+      <c r="C35" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="15">
+      <c r="B36" s="14">
         <v>2023</v>
       </c>
-      <c r="D36" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="E36" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="F36" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="I36" s="24" t="s">
-        <v>163</v>
+      <c r="C36" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>